<commit_message>
post draft I, added sample size, fixed taable, need SPELLE
</commit_message>
<xml_diff>
--- a/H03.xlsx
+++ b/H03.xlsx
@@ -12,7 +12,7 @@
     <sheet name="tab2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">flow!$A$1:$K$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">flow!$A$1:$K$22</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -54,12 +54,6 @@
     <t>high:late</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>percent</t>
-  </si>
-  <si>
     <t>completed study</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>Gen.pop</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Randomly assigned</t>
   </si>
 </sst>
 </file>
@@ -204,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -311,13 +311,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -358,6 +381,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -386,6 +410,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,342 +949,378 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+      <c r="C3" s="9">
+        <v>43426</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="C3" s="8">
-        <v>43426</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="G4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1">
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>42236</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <f>C5/C3</f>
         <v>0.9725970616681251</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="C6"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:9">
       <c r="C7"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="10">
+      <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="11">
         <v>10552</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="20">
         <v>10563</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="20">
         <v>10559</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="17">
         <v>10562</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="8">
         <v>42236</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <f>F10/C5</f>
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>16</v>
+      <c r="H10" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="14">
+      <c r="A11" s="5"/>
+      <c r="B11" s="15">
         <f>B10/$F$10</f>
         <v>0.24983426460839095</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="22">
         <f>C10/$F$10</f>
         <v>0.25009470593806232</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="22">
         <f>D10/$F$10</f>
         <v>0.25</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="19">
         <f>E10/$F$10</f>
         <v>0.25007102945354676</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <f>F10/$F$10</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1">
-      <c r="B12" s="11"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="17"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="10">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11">
         <v>10451</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="20">
         <v>10462</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="20">
         <v>10468</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="17">
         <v>10442</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="8">
         <v>41823</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <f>F13/F10</f>
         <v>0.99022161189506586</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>14</v>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5"/>
-      <c r="B14" s="14">
+      <c r="A14" s="6"/>
+      <c r="B14" s="15">
         <f>B13/$F$13</f>
         <v>0.24988642612916337</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="15">
         <f>C13/$F$13</f>
         <v>0.2501494393037324</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="15">
         <f>D13/$F$13</f>
         <v>0.25029290103531548</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="15">
         <f>E13/$F$13</f>
         <v>0.24967123353178872</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="15">
         <f>F13/$F$13</f>
         <v>1</v>
       </c>
-      <c r="G14" s="6"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="10">
+      <c r="A16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="11">
         <v>9557</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="20">
         <v>9561</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="20">
         <v>9564</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="17">
         <v>9552</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="8">
         <f>SUM(B16:E16)</f>
         <v>38234</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="7">
         <f>F16/F13</f>
         <v>0.91418597422470893</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>13</v>
+      <c r="H16" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="5"/>
-      <c r="B17" s="14">
+      <c r="A17" s="6"/>
+      <c r="B17" s="15">
         <f>B16/$F$16</f>
         <v>0.24996076790291363</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="15">
         <f>C16/$F$16</f>
         <v>0.25006538682847729</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="15">
         <f>D16/$F$16</f>
         <v>0.25014385102265002</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="15">
         <f>E16/$F$16</f>
         <v>0.24982999424595909</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="67">
         <f>F16/$F$16</f>
         <v>1</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="10">
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="6"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" s="1" customFormat="1">
+      <c r="A19" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="66">
+        <f>B13-B16</f>
+        <v>894</v>
+      </c>
+      <c r="C19" s="66">
+        <f t="shared" ref="C19:E19" si="0">C13-C16</f>
+        <v>901</v>
+      </c>
+      <c r="D19" s="66">
+        <f t="shared" si="0"/>
+        <v>904</v>
+      </c>
+      <c r="E19" s="66">
+        <f t="shared" si="0"/>
+        <v>890</v>
+      </c>
+      <c r="F19" s="66"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+    </row>
+    <row r="20" spans="1:8" s="13" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="15">
+        <f>B19/B13</f>
+        <v>8.5542053392019896E-2</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="11">
         <v>9557</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C21" s="11">
         <v>9561</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D21" s="11">
         <v>9564</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E21" s="20">
         <v>9552</v>
       </c>
-      <c r="F19" s="7">
-        <f>SUM(B19:E19)</f>
+      <c r="F21" s="8">
+        <f>SUM(B21:E21)</f>
         <v>38234</v>
       </c>
-      <c r="G19" s="6">
-        <f>F19/F16</f>
+      <c r="G21" s="7">
+        <f>F21/F16</f>
         <v>1</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="B20" s="14">
-        <f>B19/$F$16</f>
+      <c r="H21" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="B22" s="15">
+        <f>B21/$F$16</f>
         <v>0.24996076790291363</v>
       </c>
-      <c r="C20" s="14">
-        <f t="shared" ref="C20" si="0">C19/$F$16</f>
+      <c r="C22" s="15">
+        <f t="shared" ref="C22" si="1">C21/$F$16</f>
         <v>0.25006538682847729</v>
       </c>
-      <c r="D20" s="14">
-        <f t="shared" ref="D20" si="1">D19/$F$16</f>
+      <c r="D22" s="15">
+        <f t="shared" ref="D22" si="2">D21/$F$16</f>
         <v>0.25014385102265002</v>
       </c>
-      <c r="E20" s="14">
-        <f t="shared" ref="E20" si="2">E19/$F$16</f>
+      <c r="E22" s="15">
+        <f t="shared" ref="E22" si="3">E21/$F$16</f>
         <v>0.24982999424595909</v>
       </c>
-      <c r="F20" s="14">
-        <f t="shared" ref="F20" si="3">F19/$F$16</f>
+      <c r="F22" s="15">
+        <f t="shared" ref="F22" si="4">F21/$F$16</f>
         <v>1</v>
       </c>
     </row>
@@ -1271,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G17"/>
+    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1283,248 +1347,248 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9">
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="H5" s="7"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="B4" s="5" t="s">
+      <c r="C6" s="30">
+        <v>51.3</v>
+      </c>
+      <c r="D6" s="31">
+        <v>50.9</v>
+      </c>
+      <c r="E6" s="32">
+        <v>51.2</v>
+      </c>
+      <c r="F6" s="32">
+        <v>50.98</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="H5" s="6"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="C7" s="33">
+        <v>0.21</v>
+      </c>
+      <c r="D7" s="34">
+        <v>0.23</v>
+      </c>
+      <c r="E7" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="35">
+        <v>0.22</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="40">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0.16</v>
+      </c>
+      <c r="E8" s="42">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F8" s="42">
+        <v>0.15</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="43">
+        <v>0.12</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9" s="45">
+        <v>0.13</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10" s="6"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="48">
+        <v>103</v>
+      </c>
+      <c r="D11" s="49">
+        <v>105</v>
+      </c>
+      <c r="E11" s="50">
+        <v>101</v>
+      </c>
+      <c r="F11" s="50">
+        <v>107</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="30">
+        <v>24</v>
+      </c>
+      <c r="D12" s="31">
+        <v>25</v>
+      </c>
+      <c r="E12" s="32">
+        <v>27</v>
+      </c>
+      <c r="F12" s="32">
+        <v>24</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="37">
+        <v>0.08</v>
+      </c>
+      <c r="D13" s="38">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.06</v>
+      </c>
+      <c r="F13" s="39">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="48">
+        <v>18</v>
+      </c>
+      <c r="D14" s="49">
         <v>17</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="29">
-        <v>51.3</v>
-      </c>
-      <c r="D6" s="30">
-        <v>50.9</v>
-      </c>
-      <c r="E6" s="31">
-        <v>51.2</v>
-      </c>
-      <c r="F6" s="31">
-        <v>50.98</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="32">
-        <v>0.21</v>
-      </c>
-      <c r="D7" s="33">
-        <v>0.23</v>
-      </c>
-      <c r="E7" s="34">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0.22</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="38">
-        <v>0.15</v>
-      </c>
-      <c r="D8" s="39">
-        <v>0.16</v>
-      </c>
-      <c r="E8" s="40">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0.15</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="B9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="41">
-        <v>0.12</v>
-      </c>
-      <c r="D9" s="42">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E9" s="43">
-        <v>0.13</v>
-      </c>
-      <c r="F9" s="43">
-        <v>0.12</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="B10" s="5"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="46">
-        <v>103</v>
-      </c>
-      <c r="D11" s="47">
-        <v>105</v>
-      </c>
-      <c r="E11" s="48">
-        <v>101</v>
-      </c>
-      <c r="F11" s="48">
-        <v>107</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="B12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="29">
-        <v>24</v>
-      </c>
-      <c r="D12" s="30">
-        <v>25</v>
-      </c>
-      <c r="E12" s="31">
-        <v>27</v>
-      </c>
-      <c r="F12" s="31">
-        <v>24</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="35">
-        <v>0.08</v>
-      </c>
-      <c r="D13" s="36">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E13" s="37">
-        <v>0.06</v>
-      </c>
-      <c r="F13" s="37">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="46">
-        <v>18</v>
-      </c>
-      <c r="D14" s="47">
-        <v>17</v>
-      </c>
-      <c r="E14" s="48">
+      <c r="E14" s="50">
         <v>15</v>
       </c>
-      <c r="F14" s="48">
+      <c r="F14" s="50">
         <v>19</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="C15" s="15"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="46">
         <v>10552</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="46">
         <v>10563</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="46">
         <v>10559</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="46">
         <v>10562</v>
       </c>
-      <c r="G17" s="45">
+      <c r="G17" s="47">
         <v>42236</v>
       </c>
     </row>
@@ -1552,236 +1616,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10</v>
+      </c>
+      <c r="D6" s="23">
+        <v>12</v>
+      </c>
+      <c r="E6" s="51">
+        <v>17</v>
+      </c>
+      <c r="F6" s="51">
+        <v>15</v>
+      </c>
+      <c r="G6" s="61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="52">
+        <v>22</v>
+      </c>
+      <c r="D7" s="53">
+        <v>26</v>
+      </c>
+      <c r="E7" s="54">
         <v>18</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="C2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F7" s="54">
+        <v>21</v>
+      </c>
+      <c r="G7" s="62">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="55">
+        <v>36</v>
+      </c>
+      <c r="D8" s="56">
+        <v>32</v>
+      </c>
+      <c r="E8" s="57">
+        <v>38</v>
+      </c>
+      <c r="F8" s="57">
+        <v>33</v>
+      </c>
+      <c r="G8" s="63">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="6"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="63"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="52">
+        <v>27</v>
+      </c>
+      <c r="D10" s="53">
+        <v>29</v>
+      </c>
+      <c r="E10" s="54">
+        <v>31</v>
+      </c>
+      <c r="F10" s="54">
+        <v>26</v>
+      </c>
+      <c r="G10" s="62">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="58">
+        <v>52</v>
+      </c>
+      <c r="D11" s="59">
+        <v>54</v>
+      </c>
+      <c r="E11" s="60">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="13">
-        <v>10</v>
-      </c>
-      <c r="D6" s="22">
-        <v>12</v>
-      </c>
-      <c r="E6" s="49">
-        <v>17</v>
-      </c>
-      <c r="F6" s="49">
-        <v>15</v>
-      </c>
-      <c r="G6" s="59">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="50">
-        <v>22</v>
-      </c>
-      <c r="D7" s="51">
-        <v>26</v>
-      </c>
-      <c r="E7" s="52">
-        <v>18</v>
-      </c>
-      <c r="F7" s="52">
-        <v>21</v>
-      </c>
-      <c r="G7" s="60">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="53">
-        <v>36</v>
-      </c>
-      <c r="D8" s="54">
-        <v>32</v>
-      </c>
-      <c r="E8" s="55">
-        <v>38</v>
-      </c>
-      <c r="F8" s="55">
-        <v>33</v>
-      </c>
-      <c r="G8" s="61">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="5"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="61"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="F11" s="60">
+        <v>49</v>
+      </c>
+      <c r="G11" s="63">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="50">
-        <v>27</v>
-      </c>
-      <c r="D10" s="51">
-        <v>29</v>
-      </c>
-      <c r="E10" s="52">
-        <v>31</v>
-      </c>
-      <c r="F10" s="52">
-        <v>26</v>
-      </c>
-      <c r="G10" s="60">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="5" t="s">
+      <c r="C12" s="58">
+        <v>68</v>
+      </c>
+      <c r="D12" s="59">
+        <v>72</v>
+      </c>
+      <c r="E12" s="60">
+        <v>70</v>
+      </c>
+      <c r="F12" s="60">
+        <v>71</v>
+      </c>
+      <c r="G12" s="63">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="56">
-        <v>52</v>
-      </c>
-      <c r="D11" s="57">
-        <v>54</v>
-      </c>
-      <c r="E11" s="58">
-        <v>48</v>
-      </c>
-      <c r="F11" s="58">
-        <v>49</v>
-      </c>
-      <c r="G11" s="61">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="56">
-        <v>68</v>
-      </c>
-      <c r="D12" s="57">
-        <v>72</v>
-      </c>
-      <c r="E12" s="58">
-        <v>70</v>
-      </c>
-      <c r="F12" s="58">
-        <v>71</v>
-      </c>
-      <c r="G12" s="61">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="50">
+      <c r="C13" s="52">
         <v>106</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="53">
         <v>108</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="54">
         <v>110</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="54">
         <v>107</v>
       </c>
-      <c r="G13" s="60">
+      <c r="G13" s="62">
         <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="C14" s="15"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="62"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="64"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="46">
         <v>10552</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="46">
         <v>10563</v>
       </c>
-      <c r="E16" s="44">
+      <c r="E16" s="46">
         <v>10559</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="46">
         <v>10562</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="47">
         <v>42236</v>
       </c>
     </row>
@@ -1790,5 +1854,6 @@
     <mergeCell ref="C1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>